<commit_message>
Working version of Inventory Import with Genre List
</commit_message>
<xml_diff>
--- a/Excel_Mapping/Mapping/Import_Mapping_bestand.xlsx
+++ b/Excel_Mapping/Mapping/Import_Mapping_bestand.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="115">
   <si>
     <t xml:space="preserve">Rule type</t>
   </si>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">ca_collections.date</t>
   </si>
   <si>
-    <t xml:space="preserve">ca_collections</t>
+    <t xml:space="preserve">ca_collections.genre_list</t>
   </si>
   <si>
     <t xml:space="preserve">listItemSplitter</t>
@@ -97,7 +97,13 @@
     <t xml:space="preserve">{
  "delimiter": ",",
  "list": "genre_types",
- "listItemType": "^8"
+ "listItemType": "concept",
+ "relationshipType": "described",
+ "relationshipTypeDefault":"described",
+ "listItemTypeDefault":"concept",
+ "matchOn": ["idno", "labels"],
+ "ignoreParent": "1",
+ "dontCreate": "1"
 } </t>
   </si>
   <si>
@@ -147,6 +153,9 @@
   </si>
   <si>
     <t xml:space="preserve">table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ca_collections</t>
   </si>
   <si>
     <t xml:space="preserve">Sets the table for the imported data</t>
@@ -387,7 +396,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -499,6 +508,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -692,11 +708,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -807,13 +823,13 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="50.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="54"/>
@@ -918,7 +934,7 @@
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" s="4" customFormat="true" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="4" customFormat="true" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
@@ -1034,13 +1050,13 @@
         <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -1049,16 +1065,16 @@
         <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -1067,16 +1083,16 @@
         <v>24</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,13 +1100,13 @@
         <v>24</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="6"/>
@@ -1100,13 +1116,13 @@
         <v>24</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1117,13 +1133,13 @@
         <v>24</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,13 +1147,13 @@
         <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,13 +1161,13 @@
         <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1198,7 +1214,7 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -1216,39 +1232,39 @@
         <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>33</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1256,10 +1272,10 @@
         <v>24</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>13</v>
@@ -1267,180 +1283,180 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bestand Mapping & Data, Institutions Data
</commit_message>
<xml_diff>
--- a/Excel_Mapping/Mapping/Import_Mapping_bestand.xlsx
+++ b/Excel_Mapping/Mapping/Import_Mapping_bestand.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="120">
   <si>
     <t xml:space="preserve">Rule type</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">ca_collections.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"skipIfExpression":"^4 !~ /dddd-dddd/"} </t>
   </si>
   <si>
     <t xml:space="preserve">ca_collections.genre_list</t>
@@ -408,7 +411,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -517,6 +520,12 @@
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -677,7 +686,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -710,11 +719,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -826,7 +839,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -934,72 +947,75 @@
       <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="E5" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="G5" s="6"/>
     </row>
     <row r="6" s="4" customFormat="true" ht="101" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="1"/>
       <c r="F6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="8"/>
+      <c r="G6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="D10" s="1"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
@@ -1009,13 +1025,13 @@
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>10</v>
@@ -1023,141 +1039,141 @@
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="6"/>
     </row>
     <row r="16" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="12" t="s">
         <v>42</v>
       </c>
+      <c r="D16" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="E16" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1165,44 +1181,44 @@
     </row>
     <row r="21" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1263,235 +1279,235 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>69</v>
+      <c r="A2" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>28</v>
+      <c r="A3" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>75</v>
       </c>
+      <c r="C4" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="E4" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>77</v>
+      <c r="A5" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>81</v>
+      <c r="A6" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>